<commit_message>
added code for admin page
</commit_message>
<xml_diff>
--- a/src/test/resources/Automation.xlsx
+++ b/src/test/resources/Automation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\test-proj\Gold-Box_Upto-Sprint_6\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8617075E-7AC5-42E1-B0F8-F2AAD8ED7735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00A4074-A85E-4468-ABAE-CFA636905019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheme" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,14 @@
     <sheet name="Sprint-5-Categ&amp;Sub-Negative" sheetId="9" r:id="rId9"/>
     <sheet name="Sprint-6 Negative" sheetId="10" r:id="rId10"/>
     <sheet name="GoldBharat" sheetId="11" r:id="rId11"/>
+    <sheet name="GoldBharatAdminPage" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="558">
   <si>
     <t>Schemes</t>
   </si>
@@ -2147,6 +2148,21 @@
   </si>
   <si>
     <t>H.NO:118, Cnr Quality, Alwal</t>
+  </si>
+  <si>
+    <t>otp</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>AdminLoginPage</t>
+  </si>
+  <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t>4564564564</t>
   </si>
 </sst>
 </file>
@@ -2571,10 +2587,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3950,7 +3966,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3969,7 +3985,15 @@
         <v>544</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>234</v>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4021,13 +4045,56 @@
       <c r="A10" t="s">
         <v>551</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="67" t="s">
         <v>552</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{F8F0BD1E-C133-4200-838B-FA6010808FED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCCEDF3-2A7F-4F32-BD50-4A5DEBA9F762}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D102B833-4E56-4CA1-9CF6-F1D87AE34A48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5320,20 +5387,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="40" customFormat="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="42" t="s">

</xml_diff>